<commit_message>
fixed efforts and models
</commit_message>
<xml_diff>
--- a/docs/layouts.xlsx
+++ b/docs/layouts.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\ergo-layouts\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88C7EC8C-9119-4A40-85AF-00E113F751A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4888111C-E11B-4A07-88F8-636C9C9DC321}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="612" yWindow="-108" windowWidth="30216" windowHeight="17496" activeTab="1" xr2:uid="{76A7A5CA-0E08-423E-A6CA-8240103AE293}"/>
+    <workbookView xWindow="612" yWindow="-108" windowWidth="30216" windowHeight="17496" xr2:uid="{76A7A5CA-0E08-423E-A6CA-8240103AE293}"/>
   </bookViews>
   <sheets>
     <sheet name="Efforts" sheetId="1" r:id="rId1"/>
     <sheet name="Keys" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
+    <sheet name="Querty" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -92,9 +92,6 @@
     <t>v</t>
   </si>
   <si>
-    <t>"</t>
-  </si>
-  <si>
     <t>y</t>
   </si>
   <si>
@@ -149,9 +146,6 @@
     <t>/</t>
   </si>
   <si>
-    <t>\</t>
-  </si>
-  <si>
     <t>'</t>
   </si>
   <si>
@@ -174,6 +168,12 @@
   </si>
   <si>
     <t>R</t>
+  </si>
+  <si>
+    <t>\\</t>
+  </si>
+  <si>
+    <t>\"</t>
   </si>
 </sst>
 </file>
@@ -183,7 +183,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -208,6 +208,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -686,15 +694,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1007,13 +1016,17 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="30" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="6" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="20% - Accent6" xfId="3" builtinId="50"/>
     <cellStyle name="40% - Accent6" xfId="4" builtinId="51"/>
     <cellStyle name="60% - Accent6" xfId="5" builtinId="52"/>
     <cellStyle name="Accent6" xfId="2" builtinId="49"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1326,10 +1339,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463B6691-7246-46A6-9F21-3516326982E4}">
-  <dimension ref="A1:S50"/>
+  <dimension ref="A1:S51"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1463,7 +1476,7 @@
         <v>8.4</v>
       </c>
       <c r="S3" s="70" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1518,7 +1531,7 @@
         <v>10.8</v>
       </c>
       <c r="S4" s="70" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:19" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1579,7 +1592,7 @@
         <v>12.6</v>
       </c>
       <c r="S5" s="70" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1640,7 +1653,7 @@
         <v>14.4</v>
       </c>
       <c r="S6" s="70" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1661,7 +1674,7 @@
       <c r="K7" s="81"/>
       <c r="L7" s="82"/>
       <c r="S7" s="70" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -1669,668 +1682,671 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="50" t="str">
-        <f>_xlfn.TEXTJOIN(",",TRUE,D13:D50,)</f>
-        <v>"L1": 8,"L2": 7,"L3": 7,"L4": 5,"L5": 7,"L6": 8,"L7": 10,"L8": 8.4,"L9": 7.2,"L10": 6,"L11": 4,"L12": 5,"L13": 7,"L14": 8,"L15": 10.8,"L16": 5.4,"L17": 1.2,"L18": 1,"L19": 1,"L20": 6,"L21": 7,"L22": 12.6,"L23": 3.6,"L24": 3.6,"L25": 3,"L26": 3,"L27": 7,"L28": 9,"L29": 10,"L30": 14.4,"L31": 10.8,"L32": 7.2,"L33": 6,"L34": 5,"L35": 1,"L36": 3,"L37": 9,"L38": 6</v>
+        <f>_xlfn.TEXTJOIN(",",TRUE,D14:D51,)</f>
+        <v>"L1": 8,"L2": 7,"L3": 6,"L4": 5,"L5": 7,"L6": 8,"L7": 10,"L8": 8.4,"L9": 7.2,"L10": 6,"L11": 4,"L12": 5,"L13": 7,"L14": 8,"L15": 10.8,"L16": 5.4,"L17": 1.2,"L18": 1,"L19": 1,"L20": 6,"L21": 7,"L22": 12.6,"L23": 3.6,"L24": 3.6,"L25": 3,"L26": 3,"L27": 7,"L28": 9,"L29": 10,"L30": 14.4,"L31": 10.8,"L32": 7.2,"L33": 6,"L34": 5,"L35": 1,"L36": 3,"L37": 9,"L38": 6</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="50" t="str">
-        <f>_xlfn.TEXTJOIN(",",TRUE,G13:G50,)</f>
-        <v>"R1": 8,"R2": 7,"R3": 7,"R4": 5,"R5": 7,"R6": 8,"R7": 10,"R8": 8.4,"R9": 7.2,"R10": 6,"R11": 4,"R12": 5,"R13": 7,"R14": 8,"R15": 10.8,"R16": 5.4,"R17": 1.2,"R18": 1,"R19": 1,"R20": 6,"R21": 7,"R22": 12.6,"R23": 3.6,"R24": 3.6,"R25": 3,"R26": 3,"R27": 7,"R28": 9,"R29": 10,"R30": 14.4,"R31": 10.8,"R32": 7.2,"R33": 6,"R34": 5,"R35": 1,"R36": 3,"R37": 9,"R38": 6</v>
+        <f>_xlfn.TEXTJOIN(",",TRUE,G14:G51,)</f>
+        <v>"R1": 8,"R2": 7,"R3": 6,"R4": 5,"R5": 7,"R6": 8,"R7": 10,"R8": 8.4,"R9": 7.2,"R10": 6,"R11": 4,"R12": 5,"R13": 7,"R14": 8,"R15": 10.8,"R16": 5.4,"R17": 1.2,"R18": 1,"R19": 1,"R20": 6,"R21": 7,"R22": 12.6,"R23": 3.6,"R24": 3.6,"R25": 3,"R26": 3,"R27": 7,"R28": 9,"R29": 10,"R30": 14.4,"R31": 10.8,"R32": 7.2,"R33": 6,"R34": 5,"R35": 1,"R36": 3,"R37": 9,"R38": 6</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A11" s="50" t="str">
+      <c r="A11" s="50"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A12" s="50" t="str">
         <f>_xlfn.CONCAT("{",A9,",",A10,"}")</f>
-        <v>{"L1": 8,"L2": 7,"L3": 7,"L4": 5,"L5": 7,"L6": 8,"L7": 10,"L8": 8.4,"L9": 7.2,"L10": 6,"L11": 4,"L12": 5,"L13": 7,"L14": 8,"L15": 10.8,"L16": 5.4,"L17": 1.2,"L18": 1,"L19": 1,"L20": 6,"L21": 7,"L22": 12.6,"L23": 3.6,"L24": 3.6,"L25": 3,"L26": 3,"L27": 7,"L28": 9,"L29": 10,"L30": 14.4,"L31": 10.8,"L32": 7.2,"L33": 6,"L34": 5,"L35": 1,"L36": 3,"L37": 9,"L38": 6,"R1": 8,"R2": 7,"R3": 7,"R4": 5,"R5": 7,"R6": 8,"R7": 10,"R8": 8.4,"R9": 7.2,"R10": 6,"R11": 4,"R12": 5,"R13": 7,"R14": 8,"R15": 10.8,"R16": 5.4,"R17": 1.2,"R18": 1,"R19": 1,"R20": 6,"R21": 7,"R22": 12.6,"R23": 3.6,"R24": 3.6,"R25": 3,"R26": 3,"R27": 7,"R28": 9,"R29": 10,"R30": 14.4,"R31": 10.8,"R32": 7.2,"R33": 6,"R34": 5,"R35": 1,"R36": 3,"R37": 9,"R38": 6}</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A12" s="50"/>
+        <v>{"L1": 8,"L2": 7,"L3": 6,"L4": 5,"L5": 7,"L6": 8,"L7": 10,"L8": 8.4,"L9": 7.2,"L10": 6,"L11": 4,"L12": 5,"L13": 7,"L14": 8,"L15": 10.8,"L16": 5.4,"L17": 1.2,"L18": 1,"L19": 1,"L20": 6,"L21": 7,"L22": 12.6,"L23": 3.6,"L24": 3.6,"L25": 3,"L26": 3,"L27": 7,"L28": 9,"L29": 10,"L30": 14.4,"L31": 10.8,"L32": 7.2,"L33": 6,"L34": 5,"L35": 1,"L36": 3,"L37": 9,"L38": 6,"R1": 8,"R2": 7,"R3": 6,"R4": 5,"R5": 7,"R6": 8,"R7": 10,"R8": 8.4,"R9": 7.2,"R10": 6,"R11": 4,"R12": 5,"R13": 7,"R14": 8,"R15": 10.8,"R16": 5.4,"R17": 1.2,"R18": 1,"R19": 1,"R20": 6,"R21": 7,"R22": 12.6,"R23": 3.6,"R24": 3.6,"R25": 3,"R26": 3,"R27": 7,"R28": 9,"R29": 10,"R30": 14.4,"R31": 10.8,"R32": 7.2,"R33": 6,"R34": 5,"R35": 1,"R36": 3,"R37": 9,"R38": 6}</v>
+      </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A13" s="2">
+      <c r="A13" s="50"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
         <v>1</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B14" s="4">
         <f>Q2</f>
         <v>8</v>
       </c>
-      <c r="D13" s="79" t="str">
-        <f>SUBSTITUTE(_xlfn.CONCAT("""L",$A13,""": ",$B13),",",".")</f>
+      <c r="D14" s="79" t="str">
+        <f>SUBSTITUTE(_xlfn.CONCAT("""L",$A14,""": ",$B14),",",".")</f>
         <v>"L1": 8</v>
       </c>
-      <c r="G13" s="50" t="str">
-        <f>SUBSTITUTE(_xlfn.CONCAT("""R",$A13,""": ",$B13),",",".")</f>
+      <c r="G14" s="50" t="str">
+        <f>SUBSTITUTE(_xlfn.CONCAT("""R",$A14,""": ",$B14),",",".")</f>
         <v>"R1": 8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A14" s="2">
-        <v>2</v>
-      </c>
-      <c r="B14" s="4">
-        <f>P2</f>
-        <v>7</v>
-      </c>
-      <c r="D14" s="79" t="str">
-        <f t="shared" ref="D14:D50" si="0">SUBSTITUTE(_xlfn.CONCAT("""L",$A14,""": ",$B14),",",".")</f>
-        <v>"L2": 7</v>
-      </c>
-      <c r="G14" s="50" t="str">
-        <f t="shared" ref="G14:G50" si="1">SUBSTITUTE(_xlfn.CONCAT("""R",$A14,""": ",$B14),",",".")</f>
-        <v>"R2": 7</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B15" s="4">
         <f>P2</f>
         <v>7</v>
       </c>
       <c r="D15" s="79" t="str">
-        <f t="shared" si="0"/>
-        <v>"L3": 7</v>
+        <f t="shared" ref="D15:D51" si="0">SUBSTITUTE(_xlfn.CONCAT("""L",$A15,""": ",$B15),",",".")</f>
+        <v>"L2": 7</v>
       </c>
       <c r="G15" s="50" t="str">
-        <f t="shared" si="1"/>
-        <v>"R3": 7</v>
+        <f t="shared" ref="G15:G51" si="1">SUBSTITUTE(_xlfn.CONCAT("""R",$A15,""": ",$B15),",",".")</f>
+        <v>"R2": 7</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
+        <v>3</v>
+      </c>
+      <c r="B16" s="4">
+        <f>O2</f>
+        <v>6</v>
+      </c>
+      <c r="D16" s="79" t="str">
+        <f t="shared" si="0"/>
+        <v>"L3": 6</v>
+      </c>
+      <c r="G16" s="50" t="str">
+        <f t="shared" si="1"/>
+        <v>"R3": 6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
         <v>4</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B17" s="4">
         <f>N2</f>
         <v>5</v>
       </c>
-      <c r="D16" s="79" t="str">
+      <c r="D17" s="79" t="str">
         <f t="shared" si="0"/>
         <v>"L4": 5</v>
       </c>
-      <c r="G16" s="50" t="str">
+      <c r="G17" s="50" t="str">
         <f t="shared" si="1"/>
         <v>"R4": 5</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
         <v>5</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B18" s="4">
         <f>M2</f>
         <v>7</v>
       </c>
-      <c r="D17" s="79" t="str">
+      <c r="D18" s="79" t="str">
         <f t="shared" si="0"/>
         <v>"L5": 7</v>
       </c>
-      <c r="F17" s="51"/>
-      <c r="G17" s="50" t="str">
+      <c r="F18" s="51"/>
+      <c r="G18" s="50" t="str">
         <f t="shared" si="1"/>
         <v>"R5": 7</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
         <v>6</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B19" s="4">
         <f>L2</f>
         <v>8</v>
       </c>
-      <c r="D18" s="79" t="str">
+      <c r="D19" s="79" t="str">
         <f t="shared" si="0"/>
         <v>"L6": 8</v>
       </c>
-      <c r="G18" s="50" t="str">
+      <c r="G19" s="50" t="str">
         <f t="shared" si="1"/>
         <v>"R6": 8</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="2">
         <v>7</v>
       </c>
-      <c r="B19" s="4">
+      <c r="B20" s="4">
         <f>K2</f>
         <v>10</v>
       </c>
-      <c r="D19" s="79" t="str">
+      <c r="D20" s="79" t="str">
         <f t="shared" si="0"/>
         <v>"L7": 10</v>
       </c>
-      <c r="G19" s="50" t="str">
+      <c r="G20" s="50" t="str">
         <f t="shared" si="1"/>
         <v>"R7": 10</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="2">
         <v>8</v>
       </c>
-      <c r="B20" s="4">
+      <c r="B21" s="4">
         <f>Q3</f>
         <v>8.4</v>
       </c>
-      <c r="D20" s="79" t="str">
+      <c r="D21" s="79" t="str">
         <f t="shared" si="0"/>
         <v>"L8": 8.4</v>
       </c>
-      <c r="G20" s="50" t="str">
+      <c r="G21" s="50" t="str">
         <f t="shared" si="1"/>
         <v>"R8": 8.4</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="2">
         <v>9</v>
       </c>
-      <c r="B21" s="4">
+      <c r="B22" s="4">
         <f>P3</f>
         <v>7.1999999999999993</v>
       </c>
-      <c r="D21" s="79" t="str">
+      <c r="D22" s="79" t="str">
         <f t="shared" si="0"/>
         <v>"L9": 7.2</v>
       </c>
-      <c r="G21" s="50" t="str">
+      <c r="G22" s="50" t="str">
         <f t="shared" si="1"/>
         <v>"R9": 7.2</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="2">
         <v>10</v>
       </c>
-      <c r="B22" s="4">
+      <c r="B23" s="4">
         <f>O3</f>
         <v>6</v>
       </c>
-      <c r="D22" s="79" t="str">
+      <c r="D23" s="79" t="str">
         <f t="shared" si="0"/>
         <v>"L10": 6</v>
       </c>
-      <c r="G22" s="50" t="str">
+      <c r="G23" s="50" t="str">
         <f t="shared" si="1"/>
         <v>"R10": 6</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="2">
         <v>11</v>
       </c>
-      <c r="B23" s="4">
+      <c r="B24" s="4">
         <f>N3</f>
         <v>4</v>
       </c>
-      <c r="D23" s="79" t="str">
+      <c r="D24" s="79" t="str">
         <f t="shared" si="0"/>
         <v>"L11": 4</v>
       </c>
-      <c r="G23" s="50" t="str">
+      <c r="G24" s="50" t="str">
         <f t="shared" si="1"/>
         <v>"R11": 4</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="2">
         <v>12</v>
       </c>
-      <c r="B24" s="4">
+      <c r="B25" s="4">
         <f>M3</f>
         <v>5</v>
       </c>
-      <c r="D24" s="79" t="str">
+      <c r="D25" s="79" t="str">
         <f t="shared" si="0"/>
         <v>"L12": 5</v>
       </c>
-      <c r="G24" s="50" t="str">
+      <c r="G25" s="50" t="str">
         <f t="shared" si="1"/>
         <v>"R12": 5</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="2">
         <v>13</v>
       </c>
-      <c r="B25" s="4">
+      <c r="B26" s="4">
         <f>L3</f>
         <v>7</v>
       </c>
-      <c r="D25" s="79" t="str">
+      <c r="D26" s="79" t="str">
         <f t="shared" si="0"/>
         <v>"L13": 7</v>
       </c>
-      <c r="G25" s="50" t="str">
+      <c r="G26" s="50" t="str">
         <f t="shared" si="1"/>
         <v>"R13": 7</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="2">
         <v>14</v>
       </c>
-      <c r="B26" s="4">
+      <c r="B27" s="4">
         <f>K3</f>
         <v>8</v>
       </c>
-      <c r="D26" s="79" t="str">
+      <c r="D27" s="79" t="str">
         <f t="shared" si="0"/>
         <v>"L14": 8</v>
       </c>
-      <c r="G26" s="50" t="str">
+      <c r="G27" s="50" t="str">
         <f t="shared" si="1"/>
         <v>"R14": 8</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="2">
         <v>15</v>
       </c>
-      <c r="B27" s="4">
+      <c r="B28" s="4">
         <f>Q4</f>
         <v>10.8</v>
       </c>
-      <c r="D27" s="79" t="str">
+      <c r="D28" s="79" t="str">
         <f t="shared" si="0"/>
         <v>"L15": 10.8</v>
       </c>
-      <c r="G27" s="50" t="str">
+      <c r="G28" s="50" t="str">
         <f t="shared" si="1"/>
         <v>"R15": 10.8</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="2">
         <v>16</v>
       </c>
-      <c r="B28" s="4">
+      <c r="B29" s="4">
         <f>P4</f>
         <v>5.4</v>
       </c>
-      <c r="D28" s="79" t="str">
+      <c r="D29" s="79" t="str">
         <f t="shared" si="0"/>
         <v>"L16": 5.4</v>
       </c>
-      <c r="G28" s="50" t="str">
+      <c r="G29" s="50" t="str">
         <f t="shared" si="1"/>
         <v>"R16": 5.4</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="2">
         <v>17</v>
       </c>
-      <c r="B29" s="4">
+      <c r="B30" s="4">
         <f>O4</f>
         <v>1.2</v>
       </c>
-      <c r="D29" s="79" t="str">
+      <c r="D30" s="79" t="str">
         <f t="shared" si="0"/>
         <v>"L17": 1.2</v>
       </c>
-      <c r="G29" s="50" t="str">
+      <c r="G30" s="50" t="str">
         <f t="shared" si="1"/>
         <v>"R17": 1.2</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="2">
         <v>18</v>
       </c>
-      <c r="B30" s="4">
+      <c r="B31" s="4">
         <f>N4</f>
         <v>1</v>
       </c>
-      <c r="D30" s="79" t="str">
+      <c r="D31" s="79" t="str">
         <f t="shared" si="0"/>
         <v>"L18": 1</v>
       </c>
-      <c r="G30" s="50" t="str">
+      <c r="G31" s="50" t="str">
         <f t="shared" si="1"/>
         <v>"R18": 1</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="2">
         <v>19</v>
       </c>
-      <c r="B31" s="4">
+      <c r="B32" s="4">
         <f>M4</f>
         <v>1</v>
       </c>
-      <c r="D31" s="79" t="str">
+      <c r="D32" s="79" t="str">
         <f t="shared" si="0"/>
         <v>"L19": 1</v>
       </c>
-      <c r="G31" s="50" t="str">
+      <c r="G32" s="50" t="str">
         <f t="shared" si="1"/>
         <v>"R19": 1</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" s="2">
         <v>20</v>
       </c>
-      <c r="B32" s="4">
+      <c r="B33" s="4">
         <f>L4</f>
         <v>6</v>
       </c>
-      <c r="D32" s="79" t="str">
+      <c r="D33" s="79" t="str">
         <f t="shared" si="0"/>
         <v>"L20": 6</v>
       </c>
-      <c r="G32" s="50" t="str">
+      <c r="G33" s="50" t="str">
         <f t="shared" si="1"/>
         <v>"R20": 6</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" s="2">
         <v>21</v>
       </c>
-      <c r="B33" s="4">
+      <c r="B34" s="4">
         <f>K4</f>
         <v>7</v>
       </c>
-      <c r="D33" s="79" t="str">
+      <c r="D34" s="79" t="str">
         <f t="shared" si="0"/>
         <v>"L21": 7</v>
       </c>
-      <c r="G33" s="50" t="str">
+      <c r="G34" s="50" t="str">
         <f t="shared" si="1"/>
         <v>"R21": 7</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" s="2">
         <v>22</v>
       </c>
-      <c r="B34" s="4">
+      <c r="B35" s="4">
         <f>Q5</f>
         <v>12.6</v>
       </c>
-      <c r="D34" s="79" t="str">
+      <c r="D35" s="79" t="str">
         <f t="shared" si="0"/>
         <v>"L22": 12.6</v>
       </c>
-      <c r="G34" s="50" t="str">
+      <c r="G35" s="50" t="str">
         <f t="shared" si="1"/>
         <v>"R22": 12.6</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" s="2">
         <v>23</v>
       </c>
-      <c r="B35" s="4">
+      <c r="B36" s="4">
         <f>P5</f>
         <v>3.6</v>
       </c>
-      <c r="D35" s="79" t="str">
+      <c r="D36" s="79" t="str">
         <f t="shared" si="0"/>
         <v>"L23": 3.6</v>
       </c>
-      <c r="G35" s="50" t="str">
+      <c r="G36" s="50" t="str">
         <f t="shared" si="1"/>
         <v>"R23": 3.6</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" s="2">
         <v>24</v>
       </c>
-      <c r="B36" s="4">
+      <c r="B37" s="4">
         <f>O5</f>
         <v>3.5999999999999996</v>
       </c>
-      <c r="D36" s="79" t="str">
+      <c r="D37" s="79" t="str">
         <f t="shared" si="0"/>
         <v>"L24": 3.6</v>
       </c>
-      <c r="G36" s="50" t="str">
+      <c r="G37" s="50" t="str">
         <f t="shared" si="1"/>
         <v>"R24": 3.6</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" s="2">
         <v>25</v>
       </c>
-      <c r="B37" s="4">
+      <c r="B38" s="4">
         <f>N5</f>
         <v>3</v>
       </c>
-      <c r="D37" s="79" t="str">
+      <c r="D38" s="79" t="str">
         <f t="shared" si="0"/>
         <v>"L25": 3</v>
       </c>
-      <c r="G37" s="50" t="str">
+      <c r="G38" s="50" t="str">
         <f t="shared" si="1"/>
         <v>"R25": 3</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" s="2">
         <v>26</v>
       </c>
-      <c r="B38" s="4">
+      <c r="B39" s="4">
         <f>M5</f>
         <v>3</v>
       </c>
-      <c r="D38" s="79" t="str">
+      <c r="D39" s="79" t="str">
         <f t="shared" si="0"/>
         <v>"L26": 3</v>
       </c>
-      <c r="G38" s="50" t="str">
+      <c r="G39" s="50" t="str">
         <f t="shared" si="1"/>
         <v>"R26": 3</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" s="2">
         <v>27</v>
       </c>
-      <c r="B39" s="4">
+      <c r="B40" s="4">
         <f>L5</f>
         <v>7</v>
       </c>
-      <c r="D39" s="79" t="str">
+      <c r="D40" s="79" t="str">
         <f t="shared" si="0"/>
         <v>"L27": 7</v>
       </c>
-      <c r="G39" s="50" t="str">
+      <c r="G40" s="50" t="str">
         <f t="shared" si="1"/>
         <v>"R27": 7</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" s="2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" s="2">
         <v>28</v>
       </c>
-      <c r="B40" s="4">
+      <c r="B41" s="4">
         <f>K5</f>
         <v>9</v>
       </c>
-      <c r="D40" s="79" t="str">
+      <c r="D41" s="79" t="str">
         <f t="shared" si="0"/>
         <v>"L28": 9</v>
       </c>
-      <c r="G40" s="50" t="str">
+      <c r="G41" s="50" t="str">
         <f t="shared" si="1"/>
         <v>"R28": 9</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" s="2">
         <v>29</v>
       </c>
-      <c r="B41" s="4">
+      <c r="B42" s="4">
         <f>J5</f>
         <v>10</v>
       </c>
-      <c r="D41" s="79" t="str">
+      <c r="D42" s="79" t="str">
         <f t="shared" si="0"/>
         <v>"L29": 10</v>
       </c>
-      <c r="G41" s="50" t="str">
+      <c r="G42" s="50" t="str">
         <f t="shared" si="1"/>
         <v>"R29": 10</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" s="2">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43" s="2">
         <v>30</v>
       </c>
-      <c r="B42" s="4">
+      <c r="B43" s="4">
         <f>Q6</f>
         <v>14.4</v>
       </c>
-      <c r="D42" s="79" t="str">
+      <c r="D43" s="79" t="str">
         <f t="shared" si="0"/>
         <v>"L30": 14.4</v>
       </c>
-      <c r="G42" s="50" t="str">
+      <c r="G43" s="50" t="str">
         <f t="shared" si="1"/>
         <v>"R30": 14.4</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" s="2">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44" s="2">
         <v>31</v>
       </c>
-      <c r="B43" s="4">
+      <c r="B44" s="4">
         <f>P6</f>
         <v>10.8</v>
       </c>
-      <c r="D43" s="79" t="str">
+      <c r="D44" s="79" t="str">
         <f t="shared" si="0"/>
         <v>"L31": 10.8</v>
       </c>
-      <c r="G43" s="50" t="str">
+      <c r="G44" s="50" t="str">
         <f t="shared" si="1"/>
         <v>"R31": 10.8</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" s="2">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45" s="2">
         <v>32</v>
       </c>
-      <c r="B44" s="4">
+      <c r="B45" s="4">
         <f>O6</f>
         <v>7.1999999999999993</v>
       </c>
-      <c r="D44" s="79" t="str">
+      <c r="D45" s="79" t="str">
         <f t="shared" si="0"/>
         <v>"L32": 7.2</v>
       </c>
-      <c r="G44" s="50" t="str">
+      <c r="G45" s="50" t="str">
         <f t="shared" si="1"/>
         <v>"R32": 7.2</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45" s="2">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46" s="2">
         <v>33</v>
       </c>
-      <c r="B45" s="4">
+      <c r="B46" s="4">
         <f>N6</f>
         <v>6</v>
       </c>
-      <c r="D45" s="79" t="str">
+      <c r="D46" s="79" t="str">
         <f t="shared" si="0"/>
         <v>"L33": 6</v>
       </c>
-      <c r="G45" s="50" t="str">
+      <c r="G46" s="50" t="str">
         <f t="shared" si="1"/>
         <v>"R33": 6</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" s="2">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47" s="2">
         <v>34</v>
       </c>
-      <c r="B46" s="4">
+      <c r="B47" s="4">
         <f>M6</f>
         <v>5</v>
       </c>
-      <c r="D46" s="79" t="str">
+      <c r="D47" s="79" t="str">
         <f t="shared" si="0"/>
         <v>"L34": 5</v>
       </c>
-      <c r="G46" s="50" t="str">
+      <c r="G47" s="50" t="str">
         <f t="shared" si="1"/>
         <v>"R34": 5</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" s="2">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48" s="2">
         <v>35</v>
       </c>
-      <c r="B47" s="4">
+      <c r="B48" s="4">
         <f>L6</f>
         <v>1</v>
       </c>
-      <c r="D47" s="79" t="str">
+      <c r="D48" s="79" t="str">
         <f t="shared" si="0"/>
         <v>"L35": 1</v>
       </c>
-      <c r="G47" s="50" t="str">
+      <c r="G48" s="50" t="str">
         <f t="shared" si="1"/>
         <v>"R35": 1</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A48" s="2">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A49" s="2">
         <v>36</v>
       </c>
-      <c r="B48" s="4">
+      <c r="B49" s="4">
         <f>K6</f>
         <v>3</v>
       </c>
-      <c r="D48" s="79" t="str">
+      <c r="D49" s="79" t="str">
         <f t="shared" si="0"/>
         <v>"L36": 3</v>
       </c>
-      <c r="G48" s="50" t="str">
+      <c r="G49" s="50" t="str">
         <f t="shared" si="1"/>
         <v>"R36": 3</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A49" s="2">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A50" s="2">
         <v>37</v>
       </c>
-      <c r="B49" s="4">
+      <c r="B50" s="4">
         <f>J6</f>
         <v>9</v>
       </c>
-      <c r="D49" s="79" t="str">
+      <c r="D50" s="79" t="str">
         <f t="shared" si="0"/>
         <v>"L37": 9</v>
       </c>
-      <c r="G49" s="50" t="str">
+      <c r="G50" s="50" t="str">
         <f t="shared" si="1"/>
         <v>"R37": 9</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A50" s="2">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A51" s="2">
         <v>38</v>
       </c>
-      <c r="B50" s="4">
+      <c r="B51" s="4">
         <f>J7</f>
         <v>6</v>
       </c>
-      <c r="D50" s="79" t="str">
+      <c r="D51" s="79" t="str">
         <f t="shared" si="0"/>
         <v>"L38": 6</v>
       </c>
-      <c r="G50" s="50" t="str">
+      <c r="G51" s="50" t="str">
         <f t="shared" si="1"/>
         <v>"R38": 6</v>
       </c>
@@ -2351,7 +2367,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{224431CD-CF00-47DD-8ACA-64FF62A3AD19}">
   <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
@@ -2383,11 +2399,11 @@
         <v>7</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I1"/>
       <c r="J1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K1" s="95">
         <v>7</v>
@@ -2644,10 +2660,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72793DDA-B6C7-455A-9895-0EBE1A35BEFB}">
-  <dimension ref="A1:Q13"/>
+  <dimension ref="A1:Q18"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2718,30 +2734,30 @@
       <c r="H2" s="2"/>
       <c r="J2" s="27"/>
       <c r="K2" s="95" t="s">
+        <v>46</v>
+      </c>
+      <c r="L2" s="95" t="s">
         <v>19</v>
       </c>
-      <c r="L2" s="95" t="s">
-        <v>20</v>
-      </c>
       <c r="M2" s="100" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N2" s="96" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O2" s="97" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P2" s="97" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q2" s="97" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>38</v>
+      <c r="A3" s="106" t="s">
+        <v>45</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>10</v>
@@ -2763,22 +2779,22 @@
       <c r="J3" s="27"/>
       <c r="K3" s="95"/>
       <c r="L3" s="95" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M3" s="100" t="s">
         <v>1</v>
       </c>
       <c r="N3" s="96" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O3" s="97" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="P3" s="98" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q3" s="98" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
@@ -2803,19 +2819,19 @@
       <c r="J4" s="99"/>
       <c r="K4" s="99"/>
       <c r="L4" s="95" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M4" s="100" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N4" s="96" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O4" s="97" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="P4" s="98" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Q4" s="98"/>
     </row>
@@ -2832,16 +2848,16 @@
       <c r="K5" s="104"/>
       <c r="L5" s="104"/>
       <c r="M5" s="101" t="s">
+        <v>32</v>
+      </c>
+      <c r="N5" s="96" t="s">
         <v>33</v>
       </c>
-      <c r="N5" s="96" t="s">
+      <c r="O5" s="97" t="s">
         <v>34</v>
       </c>
-      <c r="O5" s="97" t="s">
+      <c r="P5" s="98" t="s">
         <v>35</v>
-      </c>
-      <c r="P5" s="98" t="s">
-        <v>36</v>
       </c>
       <c r="Q5" s="98"/>
     </row>
@@ -2952,7 +2968,7 @@
       </c>
       <c r="K9" t="str">
         <f>_xlfn.CONCAT("""",Keys!K2,""": ", """",K2,"""")</f>
-        <v>"14": """</v>
+        <v>"14": "\""</v>
       </c>
       <c r="L9" t="str">
         <f>_xlfn.CONCAT("""",Keys!L2,""": ", """",L2,"""")</f>
@@ -2982,7 +2998,7 @@
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" t="str">
         <f>_xlfn.CONCAT("""",Keys!A3,""": ", """",A3,"""")</f>
-        <v>"15": "\"</v>
+        <v>"15": "\\"</v>
       </c>
       <c r="B10" t="str">
         <f>_xlfn.CONCAT("""",Keys!B3,""": ", """",B3,"""")</f>
@@ -3170,10 +3186,6 @@
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="G13" t="str">
-        <f>_xlfn.CONCAT("""",Keys!G6,""": ", """",G6,"""")</f>
-        <v>"": ""</v>
-      </c>
       <c r="H13" t="str">
         <f>_xlfn.CONCAT("""",Keys!H6,""": ", """",H6,"""")</f>
         <v>"38": ""</v>
@@ -3183,9 +3195,30 @@
         <v>"38": ""</v>
       </c>
     </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A15" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,A8:H13,)</f>
+        <v>"1": "","2": "1","3": "2","4": "3","5": "4","6": "5","7": "","8": "","9": "q","10": "w","11": "e","12": "r","13": "t","14": "","15": "\\","16": "a","17": "s","18": "d","19": "f","20": "g","21": "","22": "","23": "z","24": "x","25": "c","26": "v","27": "b","28": "","29": "","30": "","31": "","32": "","33": "","34": "","35": "","36": "","37": "","38": ""</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A16" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,J8:Q13,)</f>
+        <v>"7": "","6": "6","5": "7","4": "8","3": "9","2": "0","1": "-","14": "\"","13": "y","12": "u","11": "i","10": "o","9": "p","8": "=","21": "","20": "h","19": "j","18": "k","17": "l","16": ";","15": "'","29": "","28": "","27": "n","26": "m","25": ",","24": ".","23": "/","22": "","37": "","36": "","35": "","34": "(","33": ")","32": "[","31": "]","30": "","38": ""</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="str">
+        <f>_xlfn.CONCAT("{","left: {",A15,"}",", right: {",A16,"}}")</f>
+        <v>{left: {"1": "","2": "1","3": "2","4": "3","5": "4","6": "5","7": "","8": "","9": "q","10": "w","11": "e","12": "r","13": "t","14": "","15": "\\","16": "a","17": "s","18": "d","19": "f","20": "g","21": "","22": "","23": "z","24": "x","25": "c","26": "v","27": "b","28": "","29": "","30": "","31": "","32": "","33": "","34": "","35": "","36": "","37": "","38": ""}, right: {"7": "","6": "6","5": "7","4": "8","3": "9","2": "0","1": "-","14": "\"","13": "y","12": "u","11": "i","10": "o","9": "p","8": "=","21": "","20": "h","19": "j","18": "k","17": "l","16": ";","15": "'","29": "","28": "","27": "n","26": "m","25": ",","24": ".","23": "/","22": "","37": "","36": "","35": "","34": "(","33": ")","32": "[","31": "]","30": "","38": ""}}</v>
+      </c>
+    </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{082F101F-1916-44E9-91C5-34C26DDAA9A5}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>